<commit_message>
add cases about txn_lsm engine
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/index/index_cases2_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/index/index_cases2_btree.xlsx
@@ -2774,18 +2774,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2800,12 +2794,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3109,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6526,7 +6519,7 @@
         <v>575</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>284</v>
@@ -7059,7 +7052,7 @@
         <v>601</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>304</v>
@@ -7182,7 +7175,7 @@
         <v>607</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>312</v>
@@ -7886,7 +7879,7 @@
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>758</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -7927,7 +7920,7 @@
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="3" t="s">
         <v>759</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -7968,7 +7961,7 @@
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>760</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -8009,7 +8002,7 @@
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>761</v>
       </c>
       <c r="B120" s="3" t="s">

</xml_diff>